<commit_message>
more Javascript, CSS, and OOPHP
</commit_message>
<xml_diff>
--- a/docs/Log.xlsx
+++ b/docs/Log.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>Nr.</t>
   </si>
@@ -249,7 +249,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D16" activeCellId="0" pane="topLeft" sqref="D16"/>
+      <selection activeCell="D25" activeCellId="0" pane="topLeft" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -566,7 +566,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="24">
       <c r="A24" s="0" t="n">
         <v>8.1</v>
       </c>
@@ -575,6 +575,9 @@
       </c>
       <c r="C24" s="0" t="s">
         <v>32</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
@@ -608,6 +611,9 @@
       </c>
       <c r="C27" s="0" t="s">
         <v>36</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="28">

</xml_diff>